<commit_message>
Data Wrangling -> Término
</commit_message>
<xml_diff>
--- a/Arquivos_de_suporte/Planejamento.xlsx
+++ b/Arquivos_de_suporte/Planejamento.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1608" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1626" uniqueCount="263">
   <si>
     <t>ano_campeonato</t>
   </si>
@@ -701,9 +701,6 @@
   </si>
   <si>
     <t>Modelamento</t>
-  </si>
-  <si>
-    <t>Verificação de relevância das variáveis explicativas</t>
   </si>
   <si>
     <t>Definir lógica para as variáveis de aproveitamento (última rodada / 3 últimas rodadas / 5 últimas rodadas)</t>
@@ -1105,17 +1102,96 @@
     <t>Batch-Fold_Index</t>
   </si>
   <si>
-    <t>Definição e incorporação no dataset da divisão de lotes/folds</t>
-  </si>
-  <si>
     <t>B</t>
+  </si>
+  <si>
+    <t>Organização das colunas do dataset</t>
+  </si>
+  <si>
+    <t>Verificação de relevância das variáveis explicativas (Máquina restrita de Boltzman? / Árvore?)</t>
+  </si>
+  <si>
+    <t>Definição do Learning Rate</t>
+  </si>
+  <si>
+    <t>Definição da Arquitetura da rede (Qtd de camadas e neurônios)</t>
+  </si>
+  <si>
+    <t>Grid Search (Ótimo Global)</t>
+  </si>
+  <si>
+    <t>Definição da Quantidade de Épocas</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Modelo de Benchmark em comparação do resultado -&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Árvore</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Definição da função de ativação -&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Sigmóide</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Definição da função custo -&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Erro Quadrático Médio</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Definição e incorporação no dataset da divisão de lotes/folds -&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Cross Validation with 5 folds</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1185,6 +1261,14 @@
       <b/>
       <sz val="14"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF0070C0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1512,7 +1596,7 @@
         <xdr:cNvPr id="6" name="Grupo 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1531,7 +1615,7 @@
           <xdr:cNvPr id="2" name="Chave direita 1" descr="8246a131-9680-40f6-ae12-ff2077c5cc7c">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1579,7 +1663,7 @@
           <xdr:cNvPr id="3" name="CaixaDeTexto 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000003000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1627,7 +1711,7 @@
           <xdr:cNvPr id="4" name="Chave direita 3" descr="906979ab-bbee-4f10-b30d-377eec01e4f5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000004000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1675,7 +1759,7 @@
           <xdr:cNvPr id="5" name="CaixaDeTexto 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000005000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2079,16 +2163,16 @@
         <v>156</v>
       </c>
       <c r="R1" s="51" t="s">
+        <v>243</v>
+      </c>
+      <c r="S1" s="51" t="s">
         <v>244</v>
       </c>
-      <c r="S1" s="51" t="s">
+      <c r="T1" s="51" t="s">
         <v>245</v>
       </c>
-      <c r="T1" s="51" t="s">
+      <c r="U1" s="51" t="s">
         <v>246</v>
-      </c>
-      <c r="U1" s="51" t="s">
-        <v>247</v>
       </c>
       <c r="V1" s="37" t="s">
         <v>0</v>
@@ -2097,13 +2181,13 @@
         <v>14</v>
       </c>
       <c r="X1" s="37" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="Y1" s="51" t="s">
+        <v>236</v>
+      </c>
+      <c r="Z1" s="51" t="s">
         <v>237</v>
-      </c>
-      <c r="Z1" s="51" t="s">
-        <v>238</v>
       </c>
       <c r="AA1" s="51" t="s">
         <v>143</v>
@@ -2253,22 +2337,22 @@
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="56" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="56" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="56" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="56" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
@@ -2283,17 +2367,17 @@
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="57" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="56" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="56" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
@@ -2403,13 +2487,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B3" s="34" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="34" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D3" s="34" t="s">
         <v>8</v>
@@ -2903,7 +2987,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>5</v>
@@ -2923,7 +3007,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>5</v>
@@ -2943,7 +3027,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>35</v>
@@ -2963,7 +3047,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>35</v>
@@ -2984,7 +3068,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>35</v>
@@ -3004,7 +3088,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>35</v>
@@ -7861,14 +7945,14 @@
   <dimension ref="A1:D60"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A28" sqref="A28"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4.140625" style="48" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="159.5703125" style="42" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="123.7109375" style="42" customWidth="1"/>
     <col min="3" max="3" width="25.42578125" style="48" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.42578125" style="48" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="42"/>
@@ -7947,7 +8031,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="44" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C6" s="45" t="s">
         <v>208</v>
@@ -7961,7 +8045,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="44" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C7" s="45" t="s">
         <v>208</v>
@@ -7975,7 +8059,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="44" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C8" s="45" t="s">
         <v>208</v>
@@ -7989,7 +8073,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="44" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C9" s="45" t="s">
         <v>208</v>
@@ -8003,7 +8087,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="44" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C10" s="45" t="s">
         <v>208</v>
@@ -8017,7 +8101,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="44" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C11" s="45" t="s">
         <v>208</v>
@@ -8031,7 +8115,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="44" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C12" s="45" t="s">
         <v>208</v>
@@ -8045,7 +8129,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="44" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C13" s="45" t="s">
         <v>208</v>
@@ -8059,7 +8143,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="44" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C14" s="45" t="s">
         <v>208</v>
@@ -8073,7 +8157,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="44" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C15" s="45" t="s">
         <v>208</v>
@@ -8087,25 +8171,27 @@
         <v>15</v>
       </c>
       <c r="B16" s="42" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C16" s="45" t="s">
         <v>208</v>
       </c>
-      <c r="D16" s="47"/>
+      <c r="D16" s="49" t="s">
+        <v>235</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="43">
         <v>16</v>
       </c>
       <c r="B17" s="44" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C17" s="45" t="s">
         <v>208</v>
       </c>
       <c r="D17" s="49" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -8113,7 +8199,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="42" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C18" s="45" t="s">
         <v>142</v>
@@ -8155,7 +8241,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="44" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C21" s="45" t="s">
         <v>142</v>
@@ -8169,7 +8255,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="44" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C22" s="45" t="s">
         <v>142</v>
@@ -8183,7 +8269,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="44" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C23" s="45" t="s">
         <v>142</v>
@@ -8197,7 +8283,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="44" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C24" s="45" t="s">
         <v>142</v>
@@ -8211,7 +8297,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="44" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C25" s="45" t="s">
         <v>142</v>
@@ -8225,7 +8311,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="44" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C26" s="45" t="s">
         <v>142</v>
@@ -8239,7 +8325,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="44" t="s">
-        <v>253</v>
+        <v>262</v>
       </c>
       <c r="C27" s="45" t="s">
         <v>142</v>
@@ -8252,32 +8338,50 @@
       <c r="A28" s="43">
         <v>27</v>
       </c>
-      <c r="B28" s="44"/>
-      <c r="C28" s="45"/>
-      <c r="D28" s="47"/>
+      <c r="B28" s="44" t="s">
+        <v>253</v>
+      </c>
+      <c r="C28" s="45" t="s">
+        <v>142</v>
+      </c>
+      <c r="D28" s="46" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="43">
         <v>28</v>
       </c>
-      <c r="B29" s="44"/>
-      <c r="C29" s="45"/>
+      <c r="B29" s="44" t="s">
+        <v>254</v>
+      </c>
+      <c r="C29" s="45" t="s">
+        <v>220</v>
+      </c>
       <c r="D29" s="47"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="43">
         <v>29</v>
       </c>
-      <c r="B30" s="44"/>
-      <c r="C30" s="45"/>
+      <c r="B30" s="44" t="s">
+        <v>259</v>
+      </c>
+      <c r="C30" s="45" t="s">
+        <v>220</v>
+      </c>
       <c r="D30" s="47"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="43">
         <v>30</v>
       </c>
-      <c r="B31" s="44"/>
-      <c r="C31" s="45"/>
+      <c r="B31" s="44" t="s">
+        <v>260</v>
+      </c>
+      <c r="C31" s="45" t="s">
+        <v>220</v>
+      </c>
       <c r="D31" s="47"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -8285,7 +8389,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="44" t="s">
-        <v>221</v>
+        <v>261</v>
       </c>
       <c r="C32" s="45" t="s">
         <v>220</v>
@@ -8296,32 +8400,48 @@
       <c r="A33" s="43">
         <v>32</v>
       </c>
-      <c r="B33" s="44"/>
-      <c r="C33" s="45"/>
+      <c r="B33" s="44" t="s">
+        <v>255</v>
+      </c>
+      <c r="C33" s="45" t="s">
+        <v>220</v>
+      </c>
       <c r="D33" s="47"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="43">
         <v>33</v>
       </c>
-      <c r="B34" s="44"/>
-      <c r="C34" s="45"/>
+      <c r="B34" s="44" t="s">
+        <v>256</v>
+      </c>
+      <c r="C34" s="45" t="s">
+        <v>220</v>
+      </c>
       <c r="D34" s="47"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="43">
         <v>34</v>
       </c>
-      <c r="B35" s="44"/>
-      <c r="C35" s="45"/>
+      <c r="B35" s="44" t="s">
+        <v>258</v>
+      </c>
+      <c r="C35" s="45" t="s">
+        <v>220</v>
+      </c>
       <c r="D35" s="47"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="43">
         <v>35</v>
       </c>
-      <c r="B36" s="44"/>
-      <c r="C36" s="45"/>
+      <c r="B36" s="44" t="s">
+        <v>257</v>
+      </c>
+      <c r="C36" s="45" t="s">
+        <v>220</v>
+      </c>
       <c r="D36" s="47"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>